<commit_message>
combine api and web
</commit_message>
<xml_diff>
--- a/test_cases/api_test_cases.xlsx
+++ b/test_cases/api_test_cases.xlsx
@@ -170,9 +170,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -215,6 +215,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -224,35 +238,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -266,39 +268,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -312,14 +292,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -338,15 +310,43 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -374,19 +374,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -398,163 +554,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -585,24 +585,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -648,11 +635,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -660,8 +660,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -685,7 +685,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0">
@@ -703,130 +703,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="5">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="4">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="7">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="8">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="3">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1181,8 +1181,8 @@
   <sheetPr/>
   <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42857142857143" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
updated web ui robot
</commit_message>
<xml_diff>
--- a/test_cases/api_test_cases.xlsx
+++ b/test_cases/api_test_cases.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>TCID</t>
   </si>
@@ -86,40 +86,43 @@
     <t>default</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>PRE_01</t>
+  </si>
+  <si>
+    <t>$[2].balance=50000.0</t>
+  </si>
+  <si>
+    <t>$[2].balance</t>
+  </si>
+  <si>
+    <t>TC001</t>
+  </si>
+  <si>
+    <t>pacs008 in cny 100</t>
+  </si>
+  <si>
+    <t>[TestSetup]PRE_01</t>
+  </si>
+  <si>
+    <t>pacs.008_inbound</t>
+  </si>
+  <si>
+    <t>j_pacs.008_in</t>
+  </si>
+  <si>
+    <t>j_pacs.008_in_cny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"amount": 100} </t>
+  </si>
+  <si>
     <t>Y</t>
   </si>
   <si>
     <t>tag1</t>
-  </si>
-  <si>
-    <t>PRE_01</t>
-  </si>
-  <si>
-    <t>$[2].balance=50000.0</t>
-  </si>
-  <si>
-    <t>$[2].balance</t>
-  </si>
-  <si>
-    <t>TC001</t>
-  </si>
-  <si>
-    <t>pacs008 in cny 100</t>
-  </si>
-  <si>
-    <t>[TestSetup]PRE_01</t>
-  </si>
-  <si>
-    <t>pacs.008_inbound</t>
-  </si>
-  <si>
-    <t>j_pacs.008_in</t>
-  </si>
-  <si>
-    <t>j_pacs.008_in_cny</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"amount": 100} </t>
   </si>
   <si>
     <t>$.amount=100.0</t>
@@ -170,9 +173,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
@@ -212,43 +215,59 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -277,6 +296,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -294,6 +320,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -303,66 +337,35 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -383,13 +386,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -401,169 +554,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -588,6 +591,30 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -631,24 +658,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -664,21 +673,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -689,143 +683,152 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1252,7 +1255,7 @@
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="K2" sqref="K2:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.41904761904762" defaultRowHeight="15"/>
@@ -1356,9 +1359,7 @@
       <c r="J2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="K2" s="3"/>
       <c r="L2" s="3">
         <v>200</v>
       </c>
@@ -1372,7 +1373,7 @@
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:19">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1389,17 +1390,15 @@
       <c r="J3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="K3" s="3"/>
       <c r="L3" s="3">
         <v>200</v>
       </c>
       <c r="M3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="6"/>
@@ -1409,46 +1408,46 @@
     </row>
     <row r="4" ht="31.5" customHeight="1" spans="1:19">
       <c r="A4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="K4" s="3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="L4" s="3">
         <v>200</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O4" s="5"/>
       <c r="P4" s="6"/>
@@ -1458,46 +1457,46 @@
     </row>
     <row r="5" ht="32.25" customHeight="1" spans="1:19">
       <c r="A5" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="L5" s="3">
         <v>200</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O5" s="5"/>
       <c r="P5" s="6"/>
@@ -1507,44 +1506,44 @@
     </row>
     <row r="6" ht="31.5" customHeight="1" spans="1:19">
       <c r="A6" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>21</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="J6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="K6" s="3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="L6" s="3">
         <v>200</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="O6" s="5"/>
       <c r="P6" s="4"/>

</xml_diff>

<commit_message>
move api configs to excel
</commit_message>
<xml_diff>
--- a/test_cases/api_test_cases.xlsx
+++ b/test_cases/api_test_cases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9144" tabRatio="500" activeTab="5"/>
+    <workbookView windowWidth="28125" windowHeight="12330" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="91">
   <si>
     <t>TCID</t>
   </si>
@@ -40,13 +40,13 @@
     <t>Headers</t>
   </si>
   <si>
-    <t>Template</t>
-  </si>
-  <si>
-    <t>Defaults</t>
-  </si>
-  <si>
-    <t>Body Modifications</t>
+    <t>Body Template</t>
+  </si>
+  <si>
+    <t>Body Default</t>
+  </si>
+  <si>
+    <t>Body User-defined Fields</t>
   </si>
   <si>
     <t>Run</t>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>j_pacs.008_in</t>
-  </si>
-  <si>
-    <t>j_pacs.008_in_cny</t>
   </si>
   <si>
     <t xml:space="preserve">{"amount": 100} </t>
@@ -135,9 +132,6 @@
   </si>
   <si>
     <t>x_pacs.008_out</t>
-  </si>
-  <si>
-    <t>x_pacs.008_out_cny</t>
   </si>
   <si>
     <t xml:space="preserve">{"amount": ${TC001.$.amount}} </t>
@@ -194,9 +188,6 @@
   </si>
   <si>
     <t>Format</t>
-  </si>
-  <si>
-    <t>pacs.008_in</t>
   </si>
   <si>
     <t>json</t>
@@ -229,9 +220,6 @@
     "address": "{{debtor.address}}"
   }
 }</t>
-  </si>
-  <si>
-    <t>pacs.008_out</t>
   </si>
   <si>
     <t>xml</t>
@@ -272,9 +260,6 @@
 &lt;/Document&gt;</t>
   </si>
   <si>
-    <t>pacs.008_in_cny</t>
-  </si>
-  <si>
     <t>{
   "transaction_id": "IN123457",
   "amount": 1500.00,
@@ -298,9 +283,6 @@
     "address": "3000 Coast City"
   }
 }</t>
-  </si>
-  <si>
-    <t>pacs.008_out_cny</t>
   </si>
   <si>
     <t>{
@@ -422,7 +404,13 @@
     <t>C:\WebDrivers\msedgedriver.exe</t>
   </si>
   <si>
-    <t>{"no-sandbox": true, "disable-dev-shm-usage": true, "disable-gpu": true, "remote-debugging-port": 9222, "headless": true}</t>
+    <t>{
+  "no-sandbox": true,
+  "disable-dev-shm-usage": true,
+  "disable-gpu": true,
+  "remote-debugging-port": 9222,
+  "headless": true
+}</t>
   </si>
   <si>
     <t>E:\Downloads\my files\chrome-win64\chrome.exe</t>
@@ -431,7 +419,12 @@
     <t>E:\Downloads\my files\chromedriver-win64\chromedriver.exe</t>
   </si>
   <si>
-    <t>{"no-sandbox": true, "disable-dev-shm-usage": true, "disable-gpu": true, "remote-debugging-port": 9222}</t>
+    <t>{
+  "no-sandbox": true,
+  "disable-dev-shm-usage": true,
+  "disable-gpu": true,
+  "remote-debugging-port": 9222
+}</t>
   </si>
 </sst>
 </file>
@@ -440,11 +433,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -459,14 +452,29 @@
     </font>
     <font>
       <sz val="10.5"/>
-      <color rgb="FF222222"/>
-      <name val="Helvetica"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10.5"/>
       <name val="Segoe UI"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -476,9 +484,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -496,6 +521,68 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -504,93 +591,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -602,30 +611,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -640,7 +627,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF7F7FA"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -652,55 +639,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -712,121 +789,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -856,30 +837,15 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -911,6 +877,32 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
@@ -919,27 +911,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -957,165 +938,159 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1507,27 +1482,27 @@
   <sheetPr/>
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.41666666666667" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.41904761904762" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.1388888888889" style="6" customWidth="1"/>
-    <col min="2" max="3" width="21.287037037037" style="6" customWidth="1"/>
-    <col min="4" max="4" width="24.7314814814815" style="6" customWidth="1"/>
-    <col min="5" max="5" width="20" style="6" customWidth="1"/>
-    <col min="6" max="6" width="8.71296296296296" style="6" customWidth="1"/>
-    <col min="7" max="7" width="17.2222222222222" style="6" customWidth="1"/>
-    <col min="8" max="8" width="18.2777777777778" style="6" customWidth="1"/>
-    <col min="9" max="9" width="38.2685185185185" style="6" customWidth="1"/>
-    <col min="10" max="10" width="5" style="6" customWidth="1"/>
-    <col min="11" max="11" width="5.57407407407407" style="6" customWidth="1"/>
-    <col min="12" max="12" width="10.5833333333333" style="6" customWidth="1"/>
-    <col min="13" max="13" width="28" style="6" customWidth="1"/>
-    <col min="14" max="14" width="26.8796296296296" style="6" customWidth="1"/>
-    <col min="15" max="1019" width="9.42592592592593" style="6"/>
-    <col min="1020" max="1020" width="9.42592592592593"/>
+    <col min="1" max="1" width="13.1428571428571" style="4" customWidth="1"/>
+    <col min="2" max="3" width="21.2857142857143" style="4" customWidth="1"/>
+    <col min="4" max="4" width="24.7333333333333" style="4" customWidth="1"/>
+    <col min="5" max="5" width="20" style="4" customWidth="1"/>
+    <col min="6" max="6" width="8.71428571428571" style="4" customWidth="1"/>
+    <col min="7" max="7" width="17.2190476190476" style="4" customWidth="1"/>
+    <col min="8" max="8" width="18.2761904761905" style="4" customWidth="1"/>
+    <col min="9" max="9" width="38.2666666666667" style="4" customWidth="1"/>
+    <col min="10" max="10" width="5" style="4" customWidth="1"/>
+    <col min="11" max="11" width="5.57142857142857" style="4" customWidth="1"/>
+    <col min="12" max="12" width="10.5809523809524" style="4" customWidth="1"/>
+    <col min="13" max="13" width="28" style="4" customWidth="1"/>
+    <col min="14" max="14" width="26.8761904761905" style="4" customWidth="1"/>
+    <col min="15" max="1019" width="9.42857142857143" style="4"/>
+    <col min="1020" max="1020" width="9.42857142857143"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:14">
@@ -1575,196 +1550,196 @@
       </c>
     </row>
     <row r="2" ht="16.5" customHeight="1" spans="1:14">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="7" t="s">
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7">
+      <c r="K2" s="5"/>
+      <c r="L2" s="5">
         <v>200</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="8"/>
+      <c r="N2" s="6"/>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:14">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="7" t="s">
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7">
+      <c r="K3" s="5"/>
+      <c r="L3" s="5">
         <v>200</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="N3" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" ht="31.5" customHeight="1" spans="1:14">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="J4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="K4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="L4" s="5">
+        <v>200</v>
+      </c>
+      <c r="M4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="L4" s="7">
+      <c r="N4" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" ht="47.25" spans="1:14">
+      <c r="A5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="5">
         <v>200</v>
       </c>
-      <c r="M4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" ht="50.4" spans="1:14">
-      <c r="A5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="7" t="s">
+      <c r="M5" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="N5" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="7" t="s">
+    </row>
+    <row r="6" ht="47.25" spans="1:14">
+      <c r="A6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="L5" s="7">
+      <c r="L6" s="5">
         <v>200</v>
       </c>
-      <c r="M5" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" ht="50.4" spans="1:14">
-      <c r="A6" s="7" t="s">
+      <c r="M6" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="N6" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="L6" s="7">
-        <v>200</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" ht="15" customHeight="1"/>
+    </row>
+    <row r="9" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1778,37 +1753,37 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="12.7777777777778" customWidth="1"/>
-    <col min="2" max="2" width="118.777777777778" customWidth="1"/>
+    <col min="1" max="1" width="12.7809523809524" customWidth="1"/>
+    <col min="2" max="2" width="118.780952380952" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.8" spans="1:2">
+    <row r="1" ht="15.75" spans="1:2">
       <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" ht="150" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="3" ht="105" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="2" ht="129.6" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" ht="86.4" spans="1:2">
-      <c r="A3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1823,46 +1798,46 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="2" width="14.7777777777778" customWidth="1"/>
-    <col min="3" max="3" width="118.777777777778" customWidth="1"/>
+    <col min="1" max="2" width="14.7809523809524" customWidth="1"/>
+    <col min="3" max="3" width="118.780952380952" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.8" spans="1:3">
+    <row r="1" ht="15.75" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" ht="269" customHeight="1" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" ht="269" customHeight="1" spans="1:3">
-      <c r="A2" s="3" t="s">
+    </row>
+    <row r="3" ht="269" customHeight="1" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" ht="269" customHeight="1" spans="1:3">
-      <c r="A3" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1876,38 +1851,38 @@
   <sheetPr/>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="17.5555555555556" customWidth="1"/>
-    <col min="2" max="2" width="118.777777777778" customWidth="1"/>
+    <col min="1" max="1" width="17.552380952381" customWidth="1"/>
+    <col min="2" max="2" width="118.780952380952" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.8" spans="1:2">
+    <row r="1" ht="15.75" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" ht="331.2" spans="1:2">
-      <c r="A2" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" ht="345.6" spans="1:2">
-      <c r="A3" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>61</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" ht="345" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" ht="360" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1922,155 +1897,155 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:D1"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="17.5555555555556" customWidth="1"/>
-    <col min="2" max="2" width="20.7777777777778" customWidth="1"/>
-    <col min="3" max="3" width="17.5555555555556" customWidth="1"/>
-    <col min="4" max="4" width="57.1111111111111" customWidth="1"/>
+    <col min="1" max="1" width="17.552380952381" customWidth="1"/>
+    <col min="2" max="2" width="20.7809523809524" customWidth="1"/>
+    <col min="3" max="3" width="17.552380952381" customWidth="1"/>
+    <col min="4" max="4" width="57.1142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.8" spans="1:4">
+    <row r="1" ht="15.75" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="3" t="s">
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="3" t="s">
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="3" t="s">
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="C10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2095,109 +2070,109 @@
   <sheetPr/>
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.11111111111111" defaultRowHeight="14.4" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9.11428571428571" defaultRowHeight="15" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="13.1111111111111" customWidth="1"/>
+    <col min="1" max="1" width="13.1142857142857" customWidth="1"/>
     <col min="2" max="2" width="8.66666666666667" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="40.4444444444444" customWidth="1"/>
+    <col min="4" max="4" width="40.447619047619" customWidth="1"/>
     <col min="5" max="5" width="21.3333333333333" customWidth="1"/>
-    <col min="6" max="6" width="18.5555555555556" customWidth="1"/>
-    <col min="7" max="7" width="24.5555555555556" customWidth="1"/>
+    <col min="6" max="6" width="18.552380952381" customWidth="1"/>
+    <col min="7" max="7" width="24.552380952381" customWidth="1"/>
     <col min="8" max="8" width="15.6666666666667" customWidth="1"/>
-    <col min="9" max="9" width="48.5555555555556" customWidth="1"/>
-    <col min="10" max="16384" width="9.11111111111111" customWidth="1"/>
+    <col min="9" max="9" width="48.552380952381" customWidth="1"/>
+    <col min="10" max="16384" width="9.11428571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.8" spans="1:9">
+    <row r="1" ht="15.75" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" ht="105" spans="1:9">
+      <c r="A2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="H2" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="2" ht="55.2" spans="1:9">
-      <c r="A2" s="2" t="s">
+      <c r="I2" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" ht="90" spans="1:9">
+      <c r="A3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" ht="55.2" spans="1:9">
-      <c r="A3" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change to body override
</commit_message>
<xml_diff>
--- a/test_cases/api_test_cases.xlsx
+++ b/test_cases/api_test_cases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9144" tabRatio="602"/>
+    <workbookView windowWidth="28125" windowHeight="12330" tabRatio="602"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <t>Body Default</t>
   </si>
   <si>
-    <t>Body User-defined Fields</t>
+    <t>Body Override</t>
   </si>
   <si>
     <t>Run</t>
@@ -366,8 +366,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -394,6 +394,11 @@
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -411,15 +416,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -431,8 +440,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -446,37 +493,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -493,7 +509,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -503,14 +518,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -532,13 +539,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -560,31 +560,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -596,19 +716,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -620,127 +728,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -770,16 +770,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -810,6 +810,32 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
@@ -817,28 +843,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -857,152 +866,143 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1419,28 +1419,28 @@
   <sheetPr/>
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.41666666666667" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.41904761904762" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.1388888888889" style="4" customWidth="1"/>
-    <col min="2" max="3" width="21.287037037037" style="4" customWidth="1"/>
-    <col min="4" max="4" width="24.7314814814815" style="4" customWidth="1"/>
+    <col min="1" max="1" width="13.1428571428571" style="4" customWidth="1"/>
+    <col min="2" max="3" width="21.2857142857143" style="4" customWidth="1"/>
+    <col min="4" max="4" width="24.7333333333333" style="4" customWidth="1"/>
     <col min="5" max="5" width="20" style="4" customWidth="1"/>
-    <col min="6" max="6" width="8.71296296296296" style="4" customWidth="1"/>
-    <col min="7" max="7" width="17.2222222222222" style="4" customWidth="1"/>
-    <col min="8" max="8" width="18.2777777777778" style="4" customWidth="1"/>
-    <col min="9" max="9" width="38.2685185185185" style="4" customWidth="1"/>
+    <col min="6" max="6" width="8.71428571428571" style="4" customWidth="1"/>
+    <col min="7" max="7" width="17.2190476190476" style="4" customWidth="1"/>
+    <col min="8" max="8" width="18.2761904761905" style="4" customWidth="1"/>
+    <col min="9" max="9" width="38.2666666666667" style="4" customWidth="1"/>
     <col min="10" max="10" width="5" style="4" customWidth="1"/>
-    <col min="11" max="11" width="5.57407407407407" style="4" customWidth="1"/>
-    <col min="12" max="12" width="10.5833333333333" style="4" customWidth="1"/>
+    <col min="11" max="11" width="5.57142857142857" style="4" customWidth="1"/>
+    <col min="12" max="12" width="10.5809523809524" style="4" customWidth="1"/>
     <col min="13" max="13" width="28" style="4" customWidth="1"/>
-    <col min="14" max="14" width="26.8796296296296" style="4" customWidth="1"/>
+    <col min="14" max="14" width="26.8761904761905" style="4" customWidth="1"/>
     <col min="15" max="15" width="9" style="5"/>
-    <col min="16" max="1019" width="9.42592592592593" style="4"/>
-    <col min="1020" max="1020" width="9.42592592592593"/>
+    <col min="16" max="1019" width="9.42857142857143" style="4"/>
+    <col min="1020" max="1020" width="9.42857142857143"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:15">
@@ -1599,7 +1599,7 @@
       </c>
       <c r="O4" s="8"/>
     </row>
-    <row r="5" ht="50.4" spans="1:15">
+    <row r="5" ht="47.25" spans="1:15">
       <c r="A5" s="6" t="s">
         <v>32</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" ht="50.4" spans="1:15">
+    <row r="6" ht="47.25" spans="1:15">
       <c r="A6" s="6" t="s">
         <v>41</v>
       </c>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="O6" s="8"/>
     </row>
-    <row r="9" ht="15" customHeight="1"/>
+    <row r="9" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1708,15 +1708,15 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="17.5555555555556" customWidth="1"/>
-    <col min="2" max="2" width="20.7777777777778" customWidth="1"/>
-    <col min="3" max="3" width="17.5555555555556" customWidth="1"/>
-    <col min="4" max="4" width="57.1111111111111" customWidth="1"/>
+    <col min="1" max="1" width="17.552380952381" customWidth="1"/>
+    <col min="2" max="2" width="20.7809523809524" customWidth="1"/>
+    <col min="3" max="3" width="17.552380952381" customWidth="1"/>
+    <col min="4" max="4" width="57.1142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.8" spans="1:4">
+    <row r="1" ht="15.75" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
@@ -1882,13 +1882,13 @@
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="12.7777777777778" customWidth="1"/>
-    <col min="2" max="2" width="118.777777777778" customWidth="1"/>
+    <col min="1" max="1" width="12.7809523809524" customWidth="1"/>
+    <col min="2" max="2" width="118.780952380952" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.8" spans="1:2">
+    <row r="1" ht="15.75" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" ht="100.8" spans="1:2">
+    <row r="2" ht="105" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" ht="57.6" spans="1:2">
+    <row r="3" ht="60" spans="1:2">
       <c r="A3" s="2" t="s">
         <v>36</v>
       </c>
@@ -1927,13 +1927,13 @@
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="2" width="14.7777777777778" customWidth="1"/>
-    <col min="3" max="3" width="118.777777777778" customWidth="1"/>
+    <col min="1" max="2" width="14.7809523809524" customWidth="1"/>
+    <col min="3" max="3" width="118.780952380952" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.8" spans="1:3">
+    <row r="1" ht="15.75" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>66</v>
       </c>
@@ -1977,17 +1977,17 @@
   <sheetPr/>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="17.5555555555556" customWidth="1"/>
-    <col min="2" max="2" width="118.777777777778" customWidth="1"/>
+    <col min="1" max="1" width="17.552380952381" customWidth="1"/>
+    <col min="2" max="2" width="118.780952380952" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.8" spans="1:2">
+    <row r="1" ht="15.75" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Optimize using saved fields
</commit_message>
<xml_diff>
--- a/test_cases/api_test_cases.xlsx
+++ b/test_cases/api_test_cases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12330" tabRatio="602"/>
+    <workbookView windowWidth="28125" windowHeight="12330" tabRatio="602" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
@@ -224,6 +224,7 @@
 timestamp: "{{timestamp}}"
 timestamp2: "{{formated_timestamp}}"
 bic: "{{bic}}"
+MyToken: "{{MyToken}}"
 user_agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/96.0.4664.93 Safari/537.36</t>
   </si>
   <si>
@@ -365,10 +366,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -387,6 +388,13 @@
       <sz val="10.5"/>
       <name val="Segoe UI"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -399,13 +407,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -416,6 +417,112 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -424,30 +531,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -457,93 +540,11 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -560,187 +561,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -769,30 +770,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -810,10 +787,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -843,11 +818,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -866,143 +847,163 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1419,8 +1420,8 @@
   <sheetPr/>
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.41904761904762" defaultRowHeight="15"/>
@@ -1705,7 +1706,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1878,8 +1879,8 @@
   <sheetPr/>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B10:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
@@ -1896,7 +1897,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" ht="105" spans="1:2">
+    <row r="2" ht="120" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -1924,7 +1925,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="2"/>
@@ -1978,7 +1979,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>

</xml_diff>

<commit_message>
removed name column from the excel
</commit_message>
<xml_diff>
--- a/test_cases/api_test_cases.xlsx
+++ b/test_cases/api_test_cases.xlsx
@@ -24,7 +24,7 @@
     <author>vhuang1</author>
   </authors>
   <commentList>
-    <comment ref="M1" authorId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -51,14 +51,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="74">
   <si>
     <t>TCID</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Descriptions</t>
   </si>
   <si>
@@ -119,7 +116,7 @@
     <t>$[2].balance</t>
   </si>
   <si>
-    <t>TC001</t>
+    <t>IB_pacs008_1</t>
   </si>
   <si>
     <t>pacs008 in cny 100</t>
@@ -147,7 +144,7 @@
 $.currency</t>
   </si>
   <si>
-    <t>TC002</t>
+    <t>OB_pacs008_1</t>
   </si>
   <si>
     <t>pacs008 out cny 100</t>
@@ -175,7 +172,7 @@
     <t>$.result.amount</t>
   </si>
   <si>
-    <t>TC003</t>
+    <t>IB_pacs008_2</t>
   </si>
   <si>
     <t>[Checkwith]Position
@@ -345,6 +342,9 @@
 &lt;/Document&gt;</t>
   </si>
   <si>
+    <t>Name</t>
+  </si>
+  <si>
     <t>{
   "transaction_id": "IN123457",
   "amount": 1500.00,
@@ -401,10 +401,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -425,9 +425,114 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <i/>
@@ -438,28 +543,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -468,9 +551,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -484,89 +574,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -574,13 +581,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
@@ -607,187 +607,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -818,9 +818,50 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -840,52 +881,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -918,138 +918,138 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1464,33 +1464,33 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M10:M11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.41904761904762" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.1428571428571" style="4" customWidth="1"/>
-    <col min="2" max="3" width="21.2857142857143" style="4" customWidth="1"/>
-    <col min="4" max="4" width="24.7333333333333" style="4" customWidth="1"/>
-    <col min="5" max="5" width="20" style="4" customWidth="1"/>
-    <col min="6" max="6" width="8.71428571428571" style="4" customWidth="1"/>
-    <col min="7" max="7" width="17.2190476190476" style="4" customWidth="1"/>
-    <col min="8" max="8" width="18.2761904761905" style="4" customWidth="1"/>
-    <col min="9" max="9" width="38.2666666666667" style="4" customWidth="1"/>
-    <col min="10" max="10" width="5" style="4" customWidth="1"/>
-    <col min="11" max="11" width="5.57142857142857" style="4" customWidth="1"/>
-    <col min="12" max="12" width="10.5809523809524" style="4" customWidth="1"/>
-    <col min="13" max="13" width="28" style="4" customWidth="1"/>
-    <col min="14" max="14" width="26.8761904761905" style="4" customWidth="1"/>
-    <col min="15" max="15" width="9" style="5"/>
-    <col min="16" max="1019" width="9.42857142857143" style="4"/>
-    <col min="1020" max="1020" width="9.42857142857143"/>
+    <col min="1" max="1" width="15" style="4" customWidth="1"/>
+    <col min="2" max="2" width="21.2857142857143" style="4" customWidth="1"/>
+    <col min="3" max="3" width="24.7333333333333" style="4" customWidth="1"/>
+    <col min="4" max="4" width="20" style="4" customWidth="1"/>
+    <col min="5" max="5" width="8.71428571428571" style="4" customWidth="1"/>
+    <col min="6" max="6" width="17.2190476190476" style="4" customWidth="1"/>
+    <col min="7" max="7" width="18.2761904761905" style="4" customWidth="1"/>
+    <col min="8" max="8" width="38.2666666666667" style="4" customWidth="1"/>
+    <col min="9" max="9" width="5" style="4" customWidth="1"/>
+    <col min="10" max="10" width="5.57142857142857" style="4" customWidth="1"/>
+    <col min="11" max="11" width="10.5809523809524" style="4" customWidth="1"/>
+    <col min="12" max="12" width="28" style="4" customWidth="1"/>
+    <col min="13" max="13" width="26.8761904761905" style="4" customWidth="1"/>
+    <col min="14" max="14" width="9" style="5"/>
+    <col min="15" max="1018" width="9.42857142857143" style="4"/>
+    <col min="1019" max="1019" width="9.42857142857143"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" spans="1:15">
+    <row r="1" ht="15.75" customHeight="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1533,80 +1533,71 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+    </row>
+    <row r="2" ht="16.5" customHeight="1" spans="1:14">
+      <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" ht="16.5" customHeight="1" spans="1:15">
-      <c r="A2" s="6" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="6"/>
+      <c r="K2" s="6">
+        <v>200</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6">
-        <v>200</v>
-      </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="7"/>
+      <c r="N2" s="8"/>
+    </row>
+    <row r="3" ht="15.75" customHeight="1" spans="1:14">
+      <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="7"/>
-      <c r="O2" s="8"/>
-    </row>
-    <row r="3" ht="15.75" customHeight="1" spans="1:15">
-      <c r="A3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="B3" s="6"/>
       <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="E3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="6"/>
+      <c r="K3" s="6">
+        <v>200</v>
+      </c>
+      <c r="L3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6">
-        <v>200</v>
-      </c>
       <c r="M3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="N3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="8"/>
+    </row>
+    <row r="4" ht="31.5" customHeight="1" spans="1:14">
+      <c r="A4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="O3" s="8"/>
-    </row>
-    <row r="4" ht="31.5" customHeight="1" spans="1:15">
-      <c r="A4" s="6" t="s">
+      <c r="B4" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>23</v>
@@ -1615,43 +1606,40 @@
         <v>24</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="7" t="s">
+      <c r="J4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="6">
+        <v>200</v>
+      </c>
+      <c r="L4" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="L4" s="6">
-        <v>200</v>
       </c>
       <c r="M4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="N4" s="8"/>
+    </row>
+    <row r="5" ht="47.25" spans="1:14">
+      <c r="A5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="O4" s="8"/>
-    </row>
-    <row r="5" ht="47.25" spans="1:15">
-      <c r="A5" s="6" t="s">
+      <c r="B5" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>32</v>
@@ -1666,77 +1654,71 @@
         <v>35</v>
       </c>
       <c r="G5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="6">
+        <v>200</v>
+      </c>
+      <c r="L5" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="L5" s="6">
-        <v>200</v>
       </c>
       <c r="M5" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="N5" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" ht="141.75" spans="1:14">
+      <c r="A6" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="O5" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" ht="141.75" spans="1:15">
-      <c r="A6" s="6" t="s">
+      <c r="B6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="7" t="s">
+      <c r="J6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="K6" s="6">
+        <v>200</v>
+      </c>
+      <c r="L6" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="L6" s="6">
-        <v>200</v>
       </c>
       <c r="M6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="N6" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="O6" s="8"/>
+      <c r="N6" s="8"/>
     </row>
     <row r="9" customHeight="1"/>
   </sheetData>
@@ -1766,142 +1748,142 @@
   <sheetData>
     <row r="1" ht="15.75" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1938,26 +1920,26 @@
   <sheetData>
     <row r="1" ht="15.75" spans="1:2">
       <c r="A1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" ht="120" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" ht="60" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1983,35 +1965,35 @@
   <sheetData>
     <row r="1" ht="15.75" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" ht="201" customHeight="1" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="3" ht="201" customHeight="1" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2037,15 +2019,15 @@
   <sheetData>
     <row r="1" ht="15.75" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" ht="201" customHeight="1" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>72</v>
@@ -2053,7 +2035,7 @@
     </row>
     <row r="3" ht="201" customHeight="1" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>73</v>

</xml_diff>

<commit_message>
change json format to yaml for body
</commit_message>
<xml_diff>
--- a/test_cases/api_test_cases.xlsx
+++ b/test_cases/api_test_cases.xlsx
@@ -14,6 +14,12 @@
     <sheet name="BodyTemplates" sheetId="3" r:id="rId4"/>
     <sheet name="BodyDefaults" sheetId="4" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="Endpoint">Endpoints[Endpoint]</definedName>
+    <definedName name="Header">Headers[HeaderName]</definedName>
+    <definedName name="BodyTemplate">BodyTemplates[TemplateName]</definedName>
+    <definedName name="BodyDefault">BodyDefaults[Name]</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
@@ -128,7 +134,7 @@
     <t>[TestSetup]PRE</t>
   </si>
   <si>
-    <t xml:space="preserve">{"amount": 100} </t>
+    <t>amount: 100</t>
   </si>
   <si>
     <t>$.amount=100.0</t>
@@ -154,10 +160,11 @@
     <t xml:space="preserve">Executes an outbound credit transfer (pacs008 out cny 100) of 100 CNY. </t>
   </si>
   <si>
-    <t>[Checkwith]Position</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"amount": ${IB_pacs008_1.$.amount}} </t>
+    <t>[CheckWith]Position</t>
+  </si>
+  <si>
+    <t>amount: ${IB_pacs008_1.$.amount}
+currency: to_uppercase(${lowercase_currency})</t>
   </si>
   <si>
     <t>$.result.amount=${IB_pacs008_1.$.amount}
@@ -180,7 +187,7 @@
   </si>
   <si>
     <t>[TestSetup]PRE
-[Checkwith]Position
+[CheckWith]Position
 [TestTeardown]PRE</t>
   </si>
   <si>
@@ -347,55 +354,43 @@
     <t>Name</t>
   </si>
   <si>
-    <t>{
-  "transaction_id": "IN123457",
-  "amount": 1500.00,
-  "currency": "CNY",
-  "debtor": {
-    "name": "Oliver Queen",
-    "phones": [
-      "555-987-1234",
-      "555-987-1235"
-    ],
-    "email": "oliver.queen@example.com",
-    "address": "500 Green Arrow Street"
-  },
-  "creditor": {
-    "name": "Hal Jordan",
-    "phones": [
-      "555-789-1234",
-      "555-789-1235"
-    ],
-    "email": "hal.jordan@example.com",
-    "address": "3000 Coast City"
-  }
-}</t>
-  </si>
-  <si>
-    <t>{
-  "InstrId": "OUT123456",
-  "EndToEndId": "E2EOUT123456",
-  "amount": 1500.00,
-  "currency": "CNY",
-  "debtor": {
-    "name": "Vick Huang",
-    "phones": [
-      "555-555-5555",
-      "555-555-5556"
-    ],
-    "email": "vick.huang@example.com",
-    "address": "600 Green Arrow Street"
-  },
-  "creditor": {
-    "name": "Jay Huang",
-    "phones": [
-      "555-666-1234",
-      "555-666-1235"
-    ],
-    "email": "jay.huang@example.com",
-    "address": "3333 Coast City"
-  }
-}</t>
+    <t>transaction_id: IN123457
+amount: 1500.00
+currency: CNY
+debtor:
+  name: Oliver Queen
+  phones:
+    - 555-987-1234
+    - 555-987-1235
+  email: oliver.queen@example.com
+  address: 500 Green Arrow Street
+creditor:
+  name: Hal Jordan
+  phones:
+    - 555-789-1234
+    - 555-789-1235
+  email: hal.jordan@example.com
+  address: 3000 Coast City</t>
+  </si>
+  <si>
+    <t>InstrId: OUT123456
+EndToEndId: E2EOUT123456
+amount: 1500.00
+currency: CNY
+debtor:
+  name: Vick Huang
+  phones:
+    - 555-555-5555
+    - 555-555-5556
+  email: vick.huang@example.com
+  address: 600 Green Arrow Street
+creditor:
+  name: Jay Huang
+  phones:
+    - 555-666-1234
+    - 555-666-1235
+  email: jay.huang@example.com
+  address: 3333 Coast City</t>
   </si>
 </sst>
 </file>
@@ -403,9 +398,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
@@ -427,6 +422,19 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -436,27 +444,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -470,6 +458,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -477,16 +472,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -500,26 +487,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -532,23 +512,38 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -562,14 +557,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -578,6 +566,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -609,43 +604,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -657,13 +700,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -675,121 +754,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -819,25 +814,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -857,17 +843,46 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -889,26 +904,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -920,138 +915,138 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1131,6 +1126,535 @@
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+        <charset val="134"/>
+        <family val="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="10"/>
+        <color auto="1"/>
+      </font>
+      <alignment vertical="center"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+        <charset val="134"/>
+        <family val="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="10"/>
+        <color auto="1"/>
+      </font>
+      <alignment vertical="center"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+        <charset val="134"/>
+        <family val="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="10"/>
+        <color auto="1"/>
+      </font>
+      <alignment vertical="center" wrapText="1"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+        <charset val="134"/>
+        <family val="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="10"/>
+        <color auto="1"/>
+      </font>
+      <alignment vertical="center" wrapText="1"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+        <charset val="134"/>
+        <family val="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="10"/>
+        <color auto="1"/>
+      </font>
+      <alignment vertical="center"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+        <charset val="134"/>
+        <family val="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="10"/>
+        <color auto="1"/>
+      </font>
+      <alignment vertical="center" wrapText="1"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+        <charset val="134"/>
+        <family val="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="10"/>
+        <color auto="1"/>
+      </font>
+      <alignment vertical="center" wrapText="1"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+        <charset val="134"/>
+        <family val="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="10"/>
+        <color auto="1"/>
+      </font>
+      <alignment vertical="center"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+        <charset val="134"/>
+        <family val="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="10"/>
+        <color auto="1"/>
+      </font>
+      <alignment vertical="center"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+        <charset val="134"/>
+        <family val="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="10"/>
+        <color auto="1"/>
+      </font>
+      <alignment vertical="center"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+        <charset val="134"/>
+        <family val="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="10"/>
+        <color auto="1"/>
+      </font>
+      <alignment vertical="center"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+        <charset val="134"/>
+        <family val="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="10"/>
+        <color auto="1"/>
+      </font>
+      <alignment vertical="center"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+        <charset val="134"/>
+        <family val="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="10"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" wrapText="1"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" wrapText="1"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" wrapText="1"/>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -1206,6 +1730,71 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:N6" totalsRowShown="0">
+  <tableColumns count="14">
+    <tableColumn id="1" name="Run" dataDxfId="0"/>
+    <tableColumn id="2" name="TCID" dataDxfId="1"/>
+    <tableColumn id="3" name="Descriptions" dataDxfId="2"/>
+    <tableColumn id="4" name="Conditions"/>
+    <tableColumn id="5" name="Body Override" dataDxfId="3"/>
+    <tableColumn id="6" name="Exp Status" dataDxfId="4"/>
+    <tableColumn id="7" name="Exp Result" dataDxfId="5"/>
+    <tableColumn id="8" name="Save Fields" dataDxfId="6"/>
+    <tableColumn id="9" name="Endpoint" dataDxfId="7"/>
+    <tableColumn id="10" name="Headers" dataDxfId="8"/>
+    <tableColumn id="11" name="Body Template" dataDxfId="9"/>
+    <tableColumn id="12" name="Body Default" dataDxfId="10"/>
+    <tableColumn id="13" name="Tags" dataDxfId="11"/>
+    <tableColumn id="14" name="Wait" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Endpoints" displayName="Endpoints" ref="A1:D10" totalsRowShown="0">
+  <tableColumns count="4">
+    <tableColumn id="1" name="Environment" dataDxfId="13"/>
+    <tableColumn id="2" name="Endpoint" dataDxfId="14"/>
+    <tableColumn id="3" name="Method" dataDxfId="15"/>
+    <tableColumn id="4" name="Path" dataDxfId="16"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Headers" displayName="Headers" ref="A1:B3" totalsRowShown="0">
+  <tableColumns count="2">
+    <tableColumn id="1" name="HeaderName" dataDxfId="17"/>
+    <tableColumn id="2" name="Content" dataDxfId="18"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="BodyTemplates" displayName="BodyTemplates" ref="A1:C3" totalsRowShown="0">
+  <tableColumns count="3">
+    <tableColumn id="1" name="TemplateName" dataDxfId="19"/>
+    <tableColumn id="2" name="Format" dataDxfId="20"/>
+    <tableColumn id="3" name="Content" dataDxfId="21"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="BodyDefaults" displayName="BodyDefaults" ref="A1:B3" totalsRowShown="0">
+  <tableColumns count="2">
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="2" name="Content"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1469,7 +2058,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.41904761904762" defaultRowHeight="15"/>
@@ -1478,9 +2067,9 @@
     <col min="2" max="2" width="15" style="4" customWidth="1"/>
     <col min="3" max="3" width="21.2857142857143" style="4" customWidth="1"/>
     <col min="4" max="4" width="19.8571428571429" style="4" customWidth="1"/>
-    <col min="5" max="5" width="38.2666666666667" style="4" customWidth="1"/>
+    <col min="5" max="5" width="42.7142857142857" style="4" customWidth="1"/>
     <col min="6" max="6" width="10.5809523809524" style="4" customWidth="1"/>
-    <col min="7" max="7" width="82.7142857142857" style="4" customWidth="1"/>
+    <col min="7" max="7" width="81" style="4" customWidth="1"/>
     <col min="8" max="8" width="26.8761904761905" style="4" customWidth="1"/>
     <col min="9" max="9" width="20" style="4" customWidth="1"/>
     <col min="10" max="10" width="8.71428571428571" style="4" customWidth="1"/>
@@ -1724,10 +2313,27 @@
     </row>
     <row r="9" customHeight="1"/>
   </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I6">
+      <formula1>Endpoint</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J6">
+      <formula1>Header</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L6">
+      <formula1>BodyDefault</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K6">
+      <formula1>BodyTemplate</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
   <legacyDrawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1737,7 +2343,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1745,7 +2351,7 @@
     <col min="1" max="1" width="17.552380952381" customWidth="1"/>
     <col min="2" max="2" width="20.7809523809524" customWidth="1"/>
     <col min="3" max="3" width="17.552380952381" customWidth="1"/>
-    <col min="4" max="4" width="57.1142857142857" customWidth="1"/>
+    <col min="4" max="4" width="66.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" spans="1:4">
@@ -1890,18 +2496,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="http://localhost:5000/api/inbound_payment.json" tooltip="http://localhost:5000/api/inbound_payment.json"/>
-    <hyperlink ref="D3" r:id="rId2" display="http://localhost:5000/api/outbound_payment.xml" tooltip="http://localhost:5000/api/outbound_payment.xml"/>
-    <hyperlink ref="D4" r:id="rId3" display="http://localhost:5000/api/positions2" tooltip="http://localhost:5000/api/positions2"/>
-    <hyperlink ref="D5" r:id="rId4" display="https://vhuang2.free.beeceptor.com/api/outbound_payment.json" tooltip="https://vhuang2.free.beeceptor.com/api/outbound_payment.json"/>
-    <hyperlink ref="D6" r:id="rId5" display="https://vhuang2.free.beeceptor.com/api/outbound_payment.xml" tooltip="https://vhuang2.free.beeceptor.com/api/outbound_payment.xml"/>
-    <hyperlink ref="D7" r:id="rId6" display="https://vhuang2.free.beeceptor.com/api/positions" tooltip="https://vhuang2.free.beeceptor.com/api/positions"/>
-    <hyperlink ref="D8" r:id="rId7" display="https://vhuang1.free.beeceptor.com/api/outbound_payment.json" tooltip="https://vhuang1.free.beeceptor.com/api/outbound_payment.json"/>
-    <hyperlink ref="D9" r:id="rId8" display="https://vhuang1.free.beeceptor.com/api/outbound_payment.xml" tooltip="https://vhuang1.free.beeceptor.com/api/outbound_payment.xml"/>
-    <hyperlink ref="D10" r:id="rId9" display="https://vhuang1.free.beeceptor.com/api/positions" tooltip="https://vhuang1.free.beeceptor.com/api/positions"/>
+    <hyperlink ref="D2" r:id="rId2" display="http://localhost:5000/api/inbound_payment.json" tooltip="http://localhost:5000/api/inbound_payment.json"/>
+    <hyperlink ref="D3" r:id="rId3" display="http://localhost:5000/api/outbound_payment.xml" tooltip="http://localhost:5000/api/outbound_payment.xml"/>
+    <hyperlink ref="D4" r:id="rId4" display="http://localhost:5000/api/positions2" tooltip="http://localhost:5000/api/positions2"/>
+    <hyperlink ref="D5" r:id="rId5" display="https://vhuang2.free.beeceptor.com/api/outbound_payment.json" tooltip="https://vhuang2.free.beeceptor.com/api/outbound_payment.json"/>
+    <hyperlink ref="D6" r:id="rId6" display="https://vhuang2.free.beeceptor.com/api/outbound_payment.xml" tooltip="https://vhuang2.free.beeceptor.com/api/outbound_payment.xml"/>
+    <hyperlink ref="D7" r:id="rId7" display="https://vhuang2.free.beeceptor.com/api/positions" tooltip="https://vhuang2.free.beeceptor.com/api/positions"/>
+    <hyperlink ref="D8" r:id="rId8" display="https://vhuang1.free.beeceptor.com/api/outbound_payment.json" tooltip="https://vhuang1.free.beeceptor.com/api/outbound_payment.json"/>
+    <hyperlink ref="D9" r:id="rId9" display="https://vhuang1.free.beeceptor.com/api/outbound_payment.xml" tooltip="https://vhuang1.free.beeceptor.com/api/outbound_payment.xml"/>
+    <hyperlink ref="D10" r:id="rId10" display="https://vhuang1.free.beeceptor.com/api/positions" tooltip="https://vhuang1.free.beeceptor.com/api/positions"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1911,12 +2520,12 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B10:B11"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="12.7809523809524" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="118.780952380952" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1947,6 +2556,9 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1956,13 +2568,13 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="2" width="14.7809523809524" customWidth="1"/>
-    <col min="3" max="3" width="118.780952380952" customWidth="1"/>
+    <col min="3" max="3" width="83.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" spans="1:3">
@@ -2001,6 +2613,9 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -2010,13 +2625,13 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="17.552380952381" customWidth="1"/>
-    <col min="2" max="2" width="118.780952380952" customWidth="1"/>
+    <col min="2" max="2" width="63.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" spans="1:2">
@@ -2046,5 +2661,8 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated e2e test cases
</commit_message>
<xml_diff>
--- a/test_cases/api_test_cases.xlsx
+++ b/test_cases/api_test_cases.xlsx
@@ -30,7 +30,7 @@
     <author>vhuang1</author>
   </authors>
   <commentList>
-    <comment ref="G1" authorId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -57,11 +57,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="77">
   <si>
     <t>Run</t>
   </si>
   <si>
+    <t>Suite</t>
+  </si>
+  <si>
     <t>TCID</t>
   </si>
   <si>
@@ -125,13 +128,16 @@
     <t>Y</t>
   </si>
   <si>
+    <t>Suite1</t>
+  </si>
+  <si>
     <t>IB_pacs008_1</t>
   </si>
   <si>
     <t xml:space="preserve">Executes an inbound credit transfer (pacs008 in cny 100) of 100 CNY. </t>
   </si>
   <si>
-    <t>[TestSetup]PRE</t>
+    <t>[SuiteSetup]PRE</t>
   </si>
   <si>
     <t>amount: 100</t>
@@ -181,6 +187,9 @@
   </si>
   <si>
     <t>x_pacs.008_out</t>
+  </si>
+  <si>
+    <t>Suite2</t>
   </si>
   <si>
     <t>IB_pacs008_2</t>
@@ -398,10 +407,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -422,43 +431,9 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -471,9 +446,20 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -487,11 +473,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -518,11 +511,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -534,14 +542,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -549,15 +549,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -572,10 +573,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Times New Roman"/>
+      <charset val="0"/>
     </font>
     <font>
       <b/>
@@ -583,11 +597,6 @@
       <name val="Times New Roman"/>
       <charset val="0"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <name val="Times New Roman"/>
-      <charset val="0"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -604,13 +613,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -622,169 +775,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -813,21 +822,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -839,6 +833,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -867,26 +870,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -902,6 +885,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -910,143 +908,154 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1733,9 +1742,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:N6" totalsRowShown="0">
-  <tableColumns count="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:O6" totalsRowShown="0">
+  <tableColumns count="15">
     <tableColumn id="1" name="Run" dataDxfId="0"/>
+    <tableColumn id="15" name="Suite"/>
     <tableColumn id="2" name="TCID" dataDxfId="1"/>
     <tableColumn id="3" name="Descriptions" dataDxfId="2"/>
     <tableColumn id="4" name="Conditions"/>
@@ -2055,33 +2065,34 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.41904761904762" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="15" style="4" customWidth="1"/>
-    <col min="3" max="3" width="21.2857142857143" style="4" customWidth="1"/>
-    <col min="4" max="4" width="19.8571428571429" style="4" customWidth="1"/>
-    <col min="5" max="5" width="42.7142857142857" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.5809523809524" style="4" customWidth="1"/>
-    <col min="7" max="7" width="81" style="4" customWidth="1"/>
-    <col min="8" max="8" width="26.8761904761905" style="4" customWidth="1"/>
-    <col min="9" max="9" width="20" style="4" customWidth="1"/>
-    <col min="10" max="10" width="8.71428571428571" style="4" customWidth="1"/>
-    <col min="11" max="11" width="17.2190476190476" style="4" customWidth="1"/>
-    <col min="12" max="12" width="18.2761904761905" style="4" customWidth="1"/>
-    <col min="13" max="13" width="5.57142857142857" style="4" customWidth="1"/>
-    <col min="14" max="14" width="9" style="5"/>
-    <col min="15" max="1017" width="9.42857142857143" style="4"/>
-    <col min="1018" max="1018" width="9.42857142857143"/>
+    <col min="2" max="2" width="7" style="4" customWidth="1"/>
+    <col min="3" max="3" width="15" style="4" customWidth="1"/>
+    <col min="4" max="4" width="21.2857142857143" style="4" customWidth="1"/>
+    <col min="5" max="5" width="19.8571428571429" style="4" customWidth="1"/>
+    <col min="6" max="6" width="42.7142857142857" style="4" customWidth="1"/>
+    <col min="7" max="7" width="10.5809523809524" style="4" customWidth="1"/>
+    <col min="8" max="8" width="81" style="4" customWidth="1"/>
+    <col min="9" max="9" width="26.8761904761905" style="4" customWidth="1"/>
+    <col min="10" max="10" width="20" style="4" customWidth="1"/>
+    <col min="11" max="11" width="8.71428571428571" style="4" customWidth="1"/>
+    <col min="12" max="12" width="17.2190476190476" style="4" customWidth="1"/>
+    <col min="13" max="13" width="18.2761904761905" style="4" customWidth="1"/>
+    <col min="14" max="14" width="5.57142857142857" style="4" customWidth="1"/>
+    <col min="15" max="15" width="9" style="5"/>
+    <col min="16" max="1018" width="9.42857142857143" style="4"/>
+    <col min="1019" max="1019" width="9.42857142857143"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" spans="1:14">
+    <row r="1" ht="15.75" customHeight="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2124,206 +2135,220 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" ht="16.5" customHeight="1" spans="1:14">
+    <row r="2" ht="16.5" customHeight="1" spans="1:15">
       <c r="A2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="6">
+      <c r="E2" s="6"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="6">
         <v>200</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>17</v>
       </c>
+      <c r="I2" s="7"/>
       <c r="J2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="6"/>
+      <c r="K2" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
-      <c r="N2" s="8"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="8"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1" spans="1:14">
+    <row r="3" ht="15.75" customHeight="1" spans="1:15">
       <c r="A3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="6">
+      <c r="E3" s="6"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="6">
         <v>200</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>16</v>
-      </c>
       <c r="H3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="6" t="s">
         <v>17</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="6"/>
+      <c r="K3" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
-      <c r="N3" s="8"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="8"/>
     </row>
-    <row r="4" ht="63" spans="1:14">
+    <row r="4" ht="63" spans="1:15">
       <c r="A4" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="6">
+        <v>200</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="8"/>
+    </row>
+    <row r="5" ht="63" spans="1:15">
+      <c r="A5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="7" t="s">
+      <c r="C5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="6">
+        <v>200</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" ht="94.5" spans="1:15">
+      <c r="A6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="6">
+      <c r="E6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="6">
         <v>200</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="6" t="s">
+      <c r="H6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="N4" s="8"/>
-    </row>
-    <row r="5" ht="63" spans="1:14">
-      <c r="A5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="K6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="M6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="6">
-        <v>200</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="N5" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" ht="94.5" spans="1:14">
-      <c r="A6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="6">
-        <v>200</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
     </row>
     <row r="9" customHeight="1"/>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J6">
       <formula1>Endpoint</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K6">
       <formula1>Header</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M6">
       <formula1>BodyDefault</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L6">
       <formula1>BodyTemplate</formula1>
     </dataValidation>
   </dataValidations>
@@ -2343,7 +2368,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A1" sqref="A1:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -2356,142 +2381,142 @@
   <sheetData>
     <row r="1" ht="15.75" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2520,7 +2545,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="A1" sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
@@ -2531,26 +2556,26 @@
   <sheetData>
     <row r="1" ht="15.75" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" ht="120" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" ht="60" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -2568,7 +2593,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="A1" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="2"/>
@@ -2579,35 +2604,35 @@
   <sheetData>
     <row r="1" ht="15.75" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" ht="201" customHeight="1" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" ht="201" customHeight="1" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2625,7 +2650,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
@@ -2636,26 +2661,26 @@
   <sheetData>
     <row r="1" ht="15.75" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" ht="201" customHeight="1" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" ht="201" customHeight="1" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add test suite structure
</commit_message>
<xml_diff>
--- a/test_cases/api_test_cases.xlsx
+++ b/test_cases/api_test_cases.xlsx
@@ -128,7 +128,7 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Suite1</t>
+    <t>API_pacs008</t>
   </si>
   <si>
     <t>IB_pacs008_1</t>
@@ -189,7 +189,7 @@
     <t>x_pacs.008_out</t>
   </si>
   <si>
-    <t>Suite2</t>
+    <t>API_pacs008_2</t>
   </si>
   <si>
     <t>IB_pacs008_2</t>
@@ -407,10 +407,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -433,21 +433,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -459,22 +445,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -490,7 +468,38 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -505,22 +514,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -534,16 +535,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -552,13 +545,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -587,9 +573,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="Times New Roman"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -597,6 +592,11 @@
       <name val="Times New Roman"/>
       <charset val="0"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Times New Roman"/>
+      <charset val="0"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -613,25 +613,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -643,61 +763,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -709,25 +781,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -739,61 +793,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -822,6 +822,39 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -837,24 +870,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -866,21 +881,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -924,142 +924,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1079,6 +1079,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2068,7 +2071,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.41904761904762" defaultRowHeight="15"/>
@@ -2166,7 +2169,7 @@
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
-      <c r="O2" s="8"/>
+      <c r="O2" s="9"/>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:15">
       <c r="A3" s="6" t="s">
@@ -2197,13 +2200,13 @@
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
-      <c r="O3" s="8"/>
+      <c r="O3" s="9"/>
     </row>
     <row r="4" ht="63" spans="1:15">
       <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -2242,13 +2245,13 @@
       <c r="N4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="O4" s="8"/>
+      <c r="O4" s="9"/>
     </row>
     <row r="5" ht="63" spans="1:15">
       <c r="A5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -2287,7 +2290,7 @@
       <c r="N5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="O5" s="8">
+      <c r="O5" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2295,7 +2298,7 @@
       <c r="A6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="8" t="s">
         <v>42</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -2334,7 +2337,7 @@
       <c r="N6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="O6" s="8"/>
+      <c r="O6" s="9"/>
     </row>
     <row r="9" customHeight="1"/>
   </sheetData>

</xml_diff>